<commit_message>
Added probability distributions to figures. STILL NEED TO CHANGE TEXT
</commit_message>
<xml_diff>
--- a/Abbreviations.xlsx
+++ b/Abbreviations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blandt/Desktop/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4561B58A-735D-8942-8381-07CEE73145BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56ACC3F-FC8E-FD40-99AE-3D03FABDA75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{EE4004A4-201F-C64C-905D-C2D5B0EC0D9E}"/>
   </bookViews>
@@ -545,7 +545,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>